<commit_message>
Task list show Individual column
</commit_message>
<xml_diff>
--- a/Staff-2020-08-07.xlsx
+++ b/Staff-2020-08-07.xlsx
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Start Date: 2020-08-05, End Date: 2020-08-10, Staff name: Aser</t>
+          <t xml:space="preserve">Start Date: 2020-08-05, End Date: 2020-08-07, Staff name: </t>
         </is>
       </c>
     </row>
@@ -504,35 +504,35 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Aser</t>
+          <t>Kidden</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2020-08-10</t>
+          <t>2020-08-07</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">entryname No. 4 on </t>
+          <t xml:space="preserve">entryname No. 2 on </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>05 : 29</t>
+          <t>01 : 41</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>02 : 24</t>
+          <t>00 : 40</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>7.88</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="6">

</xml_diff>